<commit_message>
Add update query statement
</commit_message>
<xml_diff>
--- a/init/modul.xlsx
+++ b/init/modul.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICRAF\Kodingan\cdna\init\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MRV-MMI\Apps\cda\init\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDDDF56-E0B2-4D2F-8B22-62C11A26D9A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C347B64F-7E21-4CEF-BBF5-36F8D6025F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="4" xr2:uid="{C090D78D-80EC-4C5C-8D70-23CBA09D23ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C090D78D-80EC-4C5C-8D70-23CBA09D23ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Energi" sheetId="6" r:id="rId1"/>
@@ -74,12 +74,6 @@
     <t>Aksi mitigasi subsektor Pertanian</t>
   </si>
   <si>
-    <t>Aksi mitigasi subesektor energi</t>
-  </si>
-  <si>
-    <t>Aksi mitigasi subesektor transportasi</t>
-  </si>
-  <si>
     <t>Aksi mitigasi sektor pengelolaan limbah</t>
   </si>
   <si>
@@ -105,6 +99,12 @@
   </si>
   <si>
     <t>Skenario Pembangunan Rendah Karbon</t>
+  </si>
+  <si>
+    <t>Aksi mitigasi subsektor transportasi</t>
+  </si>
+  <si>
+    <t>Aksi mitigasi subsektor energi</t>
   </si>
 </sst>
 </file>
@@ -520,83 +520,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D73E2C-1528-4902-B416-9D7586F2F235}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -609,82 +609,82 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -697,82 +697,82 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -785,82 +785,82 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -872,83 +872,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FE4FB2-28CB-4472-BB3D-15B668BEE3B2}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -961,72 +961,72 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1039,72 +1039,72 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.88671875" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>